<commit_message>
mostly working but needs work on bias constraints
</commit_message>
<xml_diff>
--- a/caps.xlsx
+++ b/caps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\18312\Desktop\214A\EE214A_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D0840B-A623-4135-AA63-611AABA447C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881EE9B2-0F9A-4E0D-8D76-C8DBFC25FACD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-210" yWindow="150" windowWidth="14115" windowHeight="15150" activeTab="1" xr2:uid="{D8206649-F15A-48C4-9489-3F62BFEEAB35}"/>
+    <workbookView xWindow="9480" yWindow="510" windowWidth="17970" windowHeight="14940" activeTab="1" xr2:uid="{D8206649-F15A-48C4-9489-3F62BFEEAB35}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="22">
   <si>
     <t>Cgs</t>
   </si>
@@ -5098,6 +5098,2588 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000B-6790-4408-BC40-B7F7036167B1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="446262768"/>
+        <c:axId val="446266288"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="446262768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>W [um]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="446266288"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="446266288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="250"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>C</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> [fF]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="446262768"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>pmos</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>, L=4u</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>nmos_1u!$AK$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>cgs [fF]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.33678327184512086"/>
+                  <c:y val="2.8769228617954803E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="#,##0.000" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>nmos_1u!$AL$1:$AQ$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>nmos_1u!$AL$6:$AQ$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>13.2667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>33.166800000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>66.333600000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>132.66730000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>331.66820000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>663.33640000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2F81-4954-B83D-9592CAAD0545}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>nmos_1u!$AK$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>cgd [fF]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.0870097748463781E-4"/>
+                  <c:y val="1.444067460494017E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="#,##0.000" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>nmos_1u!$AL$1:$AQ$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>nmos_1u!$AL$7:$AQ$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.0123</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5306999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0613000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.1227</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25.306699999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50.613300000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-2F81-4954-B83D-9592CAAD0545}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>nmos_1u!$AK$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>cgb [fF]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="#,##0.000" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>nmos_1u!$AL$1:$AQ$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>nmos_1u!$AL$8:$AQ$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.22010000000000018</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5501999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.100399999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.200599999999989</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.5017000000000067</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.00350000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-2F81-4954-B83D-9592CAAD0545}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>nmos_1u!$AK$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>csb [fF]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.8992992123182044E-3"/>
+                  <c:y val="4.1049102971704172E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="#,##0.000" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>nmos_1u!$AL$1:$AQ$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>nmos_1u!$AL$9:$AQ$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>4.6000000000000014</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.3500000000000014</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>27.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64.599999999999966</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>127.10000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-2F81-4954-B83D-9592CAAD0545}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>nmos_1u!$AK$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>cdb [fF]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.0870097748463781E-4"/>
+                  <c:y val="8.2806014850257986E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="#,##0.000" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>nmos_1u!$AL$1:$AQ$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>nmos_1u!$AL$10:$AQ$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3.8923000000000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.9908999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.1555</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22.484400000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>53.471399999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>105.1164</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-2F81-4954-B83D-9592CAAD0545}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>nmos_1u!$AB$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>cgs_calc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.22143726719495124"/>
+                  <c:y val="0.14177966651115548"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="#,##0.000" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>nmos_1u!$AL$1:$AQ$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>nmos_1u!$AL$11:$AQ$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>12.266666666666666</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30.666666666666664</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>61.333333333333329</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>122.66666666666666</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>306.66666666666663</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>613.33333333333326</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-2F81-4954-B83D-9592CAAD0545}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="446262768"/>
+        <c:axId val="446266288"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="446262768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>W [um]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="446266288"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="446266288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="250"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>C</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> [fF]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="446262768"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>pmos</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>, L=4u</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>nmos_1u!$AK$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>cgs [fF]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.33678327184512086"/>
+                  <c:y val="2.8769228617954803E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="#,##0.000" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>nmos_1u!$AL$1:$AQ$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>nmos_1u!$AL$6:$AQ$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>13.2667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>33.166800000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>66.333600000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>132.66730000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>331.66820000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>663.33640000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3021-4664-985F-02746BAA8231}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>nmos_1u!$AK$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>cgd [fF]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.0870097748463781E-4"/>
+                  <c:y val="1.444067460494017E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="#,##0.000" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>nmos_1u!$AL$1:$AQ$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>nmos_1u!$AL$7:$AQ$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.0123</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5306999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0613000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.1227</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25.306699999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50.613300000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-3021-4664-985F-02746BAA8231}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>nmos_1u!$AK$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>cgb [fF]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="#,##0.000" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>nmos_1u!$AL$1:$AQ$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>nmos_1u!$AL$8:$AQ$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.22010000000000018</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5501999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.100399999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.200599999999989</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.5017000000000067</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.00350000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-3021-4664-985F-02746BAA8231}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>nmos_1u!$AK$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>csb [fF]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.8992992123182044E-3"/>
+                  <c:y val="4.1049102971704172E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="#,##0.000" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>nmos_1u!$AL$1:$AQ$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>nmos_1u!$AL$9:$AQ$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>4.6000000000000014</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.3500000000000014</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>27.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64.599999999999966</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>127.10000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-3021-4664-985F-02746BAA8231}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>nmos_1u!$AK$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>cdb [fF]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.0870097748463781E-4"/>
+                  <c:y val="8.2806014850257986E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="#,##0.000" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>nmos_1u!$AL$1:$AQ$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>nmos_1u!$AL$10:$AQ$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3.8923000000000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.9908999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.1555</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22.484400000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>53.471399999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>105.1164</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-3021-4664-985F-02746BAA8231}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>nmos_1u!$AB$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>cgs_calc</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.22143726719495124"/>
+                  <c:y val="0.14177966651115548"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="#,##0.000" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>nmos_1u!$AL$1:$AQ$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>nmos_1u!$AL$11:$AQ$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>12.266666666666666</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30.666666666666664</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>61.333333333333329</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>122.66666666666666</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>306.66666666666663</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>613.33333333333326</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-3021-4664-985F-02746BAA8231}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5596,6 +8178,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -7145,6 +9807,1038 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7807,6 +11501,82 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>22412</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>22411</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>576543</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>145676</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2C0143E-9850-49DB-AFCC-6740DD6278D9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>45</xdr:col>
+      <xdr:colOff>22411</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>22412</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>53</xdr:col>
+      <xdr:colOff>576542</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>145677</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C85723D6-A92D-45E2-9147-539A2988DA14}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -8160,15 +11930,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59410281-FCCE-4CDD-AA76-884E080700AA}">
-  <dimension ref="A1:AH39"/>
+  <dimension ref="A1:AZ39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AB34" sqref="AB34:AD39"/>
+    <sheetView tabSelected="1" topLeftCell="AH1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AS9" sqref="AS9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>12</v>
       </c>
@@ -8253,8 +12023,50 @@
       <c r="AH1" s="7">
         <v>100</v>
       </c>
+      <c r="AK1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL1" s="6">
+        <v>2</v>
+      </c>
+      <c r="AM1" s="6">
+        <v>5</v>
+      </c>
+      <c r="AN1" s="6">
+        <v>10</v>
+      </c>
+      <c r="AO1" s="6">
+        <v>20</v>
+      </c>
+      <c r="AP1" s="6">
+        <v>50</v>
+      </c>
+      <c r="AQ1" s="7">
+        <v>100</v>
+      </c>
+      <c r="AT1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="AU1" s="6">
+        <v>2</v>
+      </c>
+      <c r="AV1" s="6">
+        <v>5</v>
+      </c>
+      <c r="AW1" s="6">
+        <v>10</v>
+      </c>
+      <c r="AX1" s="6">
+        <v>20</v>
+      </c>
+      <c r="AY1" s="6">
+        <v>50</v>
+      </c>
+      <c r="AZ1" s="7">
+        <v>100</v>
+      </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -8339,8 +12151,38 @@
       <c r="AH2" s="18">
         <v>155.42310000000001</v>
       </c>
+      <c r="AK2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL2" s="16">
+        <v>4.9046000000000003</v>
+      </c>
+      <c r="AM2" s="17">
+        <v>9.5215999999999994</v>
+      </c>
+      <c r="AN2" s="17">
+        <v>17.216799999999999</v>
+      </c>
+      <c r="AO2" s="17">
+        <v>32.607100000000003</v>
+      </c>
+      <c r="AP2" s="17">
+        <v>78.778099999999995</v>
+      </c>
+      <c r="AQ2" s="18">
+        <v>155.72970000000001</v>
+      </c>
+      <c r="AT2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AU2" s="16"/>
+      <c r="AV2" s="17"/>
+      <c r="AW2" s="17"/>
+      <c r="AX2" s="17"/>
+      <c r="AY2" s="17"/>
+      <c r="AZ2" s="18"/>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
@@ -8425,8 +12267,38 @@
       <c r="AH3" s="21">
         <v>412.47660000000002</v>
       </c>
+      <c r="AK3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AL3" s="19">
+        <v>14.4991</v>
+      </c>
+      <c r="AM3" s="20">
+        <v>36.247700000000002</v>
+      </c>
+      <c r="AN3" s="20">
+        <v>72.4953</v>
+      </c>
+      <c r="AO3" s="20">
+        <v>144.9906</v>
+      </c>
+      <c r="AP3" s="20">
+        <v>362.47660000000002</v>
+      </c>
+      <c r="AQ3" s="21">
+        <v>724.95320000000004</v>
+      </c>
+      <c r="AT3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AU3" s="19"/>
+      <c r="AV3" s="20"/>
+      <c r="AW3" s="20"/>
+      <c r="AX3" s="20"/>
+      <c r="AY3" s="20"/>
+      <c r="AZ3" s="21"/>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
@@ -8511,8 +12383,38 @@
       <c r="AH4" s="21">
         <v>483.76819999999998</v>
       </c>
+      <c r="AK4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AL4" s="19">
+        <v>17.866700000000002</v>
+      </c>
+      <c r="AM4" s="20">
+        <v>41.516800000000003</v>
+      </c>
+      <c r="AN4" s="20">
+        <v>80.933599999999998</v>
+      </c>
+      <c r="AO4" s="20">
+        <v>159.76730000000001</v>
+      </c>
+      <c r="AP4" s="20">
+        <v>396.26819999999998</v>
+      </c>
+      <c r="AQ4" s="21">
+        <v>790.43640000000005</v>
+      </c>
+      <c r="AT4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AU4" s="19"/>
+      <c r="AV4" s="20"/>
+      <c r="AW4" s="20"/>
+      <c r="AX4" s="20"/>
+      <c r="AY4" s="20"/>
+      <c r="AZ4" s="21"/>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
@@ -8597,8 +12499,38 @@
       <c r="AH5" s="21">
         <v>237.71809999999999</v>
       </c>
+      <c r="AK5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL5" s="19">
+        <v>8.7124000000000006</v>
+      </c>
+      <c r="AM5" s="20">
+        <v>15.8912</v>
+      </c>
+      <c r="AN5" s="20">
+        <v>27.855799999999999</v>
+      </c>
+      <c r="AO5" s="20">
+        <v>51.785200000000003</v>
+      </c>
+      <c r="AP5" s="20">
+        <v>123.5732</v>
+      </c>
+      <c r="AQ5" s="21">
+        <v>243.2199</v>
+      </c>
+      <c r="AT5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AU5" s="19"/>
+      <c r="AV5" s="20"/>
+      <c r="AW5" s="20"/>
+      <c r="AX5" s="20"/>
+      <c r="AY5" s="20"/>
+      <c r="AZ5" s="21"/>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -8683,8 +12615,38 @@
       <c r="AH6" s="18">
         <v>356.66820000000001</v>
       </c>
+      <c r="AK6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AL6" s="16">
+        <v>13.2667</v>
+      </c>
+      <c r="AM6" s="17">
+        <v>33.166800000000002</v>
+      </c>
+      <c r="AN6" s="17">
+        <v>66.333600000000004</v>
+      </c>
+      <c r="AO6" s="17">
+        <v>132.66730000000001</v>
+      </c>
+      <c r="AP6" s="17">
+        <v>331.66820000000001</v>
+      </c>
+      <c r="AQ6" s="18">
+        <v>663.33640000000003</v>
+      </c>
+      <c r="AT6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AU6" s="16"/>
+      <c r="AV6" s="17"/>
+      <c r="AW6" s="17"/>
+      <c r="AX6" s="17"/>
+      <c r="AY6" s="17"/>
+      <c r="AZ6" s="18"/>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
@@ -8769,8 +12731,38 @@
       <c r="AH7" s="21">
         <v>50.306699999999999</v>
       </c>
+      <c r="AK7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="AL7" s="19">
+        <v>1.0123</v>
+      </c>
+      <c r="AM7" s="20">
+        <v>2.5306999999999999</v>
+      </c>
+      <c r="AN7" s="20">
+        <v>5.0613000000000001</v>
+      </c>
+      <c r="AO7" s="20">
+        <v>10.1227</v>
+      </c>
+      <c r="AP7" s="20">
+        <v>25.306699999999999</v>
+      </c>
+      <c r="AQ7" s="21">
+        <v>50.613300000000002</v>
+      </c>
+      <c r="AT7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="AU7" s="19"/>
+      <c r="AV7" s="20"/>
+      <c r="AW7" s="20"/>
+      <c r="AX7" s="20"/>
+      <c r="AY7" s="20"/>
+      <c r="AZ7" s="21"/>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>19</v>
       </c>
@@ -8879,8 +12871,62 @@
         <f t="shared" ref="AH8" si="11">AH3-AH6-AH7</f>
         <v>5.5017000000000067</v>
       </c>
+      <c r="AK8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AL8" s="16">
+        <f>AL3-AL6-AL7</f>
+        <v>0.22010000000000018</v>
+      </c>
+      <c r="AM8" s="17">
+        <f t="shared" ref="AM8:AQ8" si="12">AM3-AM6-AM7</f>
+        <v>0.5501999999999998</v>
+      </c>
+      <c r="AN8" s="17">
+        <f t="shared" si="12"/>
+        <v>1.100399999999996</v>
+      </c>
+      <c r="AO8" s="17">
+        <f t="shared" si="12"/>
+        <v>2.200599999999989</v>
+      </c>
+      <c r="AP8" s="17">
+        <f t="shared" si="12"/>
+        <v>5.5017000000000067</v>
+      </c>
+      <c r="AQ8" s="18">
+        <f t="shared" si="12"/>
+        <v>11.00350000000001</v>
+      </c>
+      <c r="AT8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AU8" s="16">
+        <f>AU3-AU6-AU7</f>
+        <v>0</v>
+      </c>
+      <c r="AV8" s="17">
+        <f t="shared" ref="AV8:AZ8" si="13">AV3-AV6-AV7</f>
+        <v>0</v>
+      </c>
+      <c r="AW8" s="17">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AX8" s="17">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AY8" s="17">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AZ8" s="18">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>20</v>
       </c>
@@ -8889,23 +12935,23 @@
         <v>4.6000000000000005</v>
       </c>
       <c r="C9" s="20">
-        <f t="shared" ref="C9:G9" si="12">C4-C6</f>
+        <f t="shared" ref="C9:G9" si="14">C4-C6</f>
         <v>6.9999999999999982</v>
       </c>
       <c r="D9" s="20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>11</v>
       </c>
       <c r="E9" s="20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>19</v>
       </c>
       <c r="F9" s="20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>42.999899999999997</v>
       </c>
       <c r="G9" s="21">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>82.999999999999972</v>
       </c>
       <c r="J9" s="3" t="s">
@@ -8916,23 +12962,23 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="L9" s="20">
-        <f t="shared" ref="L9:P9" si="13">L4-L6</f>
+        <f t="shared" ref="L9:P9" si="15">L4-L6</f>
         <v>7</v>
       </c>
       <c r="M9" s="20">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>11</v>
       </c>
       <c r="N9" s="20">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>19</v>
       </c>
       <c r="O9" s="20">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>43</v>
       </c>
       <c r="P9" s="21">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>83</v>
       </c>
       <c r="S9" s="3" t="s">
@@ -8943,23 +12989,23 @@
         <v>4.6000000000000005</v>
       </c>
       <c r="U9" s="20">
-        <f t="shared" ref="U9:Y9" si="14">U4-U6</f>
+        <f t="shared" ref="U9:Y9" si="16">U4-U6</f>
         <v>8.35</v>
       </c>
       <c r="V9" s="20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>14.599999999999998</v>
       </c>
       <c r="W9" s="20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>27.1</v>
       </c>
       <c r="X9" s="20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>64.599899999999991</v>
       </c>
       <c r="Y9" s="21">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>127.1</v>
       </c>
       <c r="AB9" s="3" t="s">
@@ -8970,27 +13016,81 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="AD9" s="20">
-        <f t="shared" ref="AD9:AH9" si="15">AD4-AD6</f>
+        <f t="shared" ref="AD9:AH9" si="17">AD4-AD6</f>
         <v>8.3499999999999979</v>
       </c>
       <c r="AE9" s="20">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>14.600000000000001</v>
       </c>
       <c r="AF9" s="20">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>27.099999999999994</v>
       </c>
       <c r="AG9" s="20">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>64.599999999999994</v>
       </c>
       <c r="AH9" s="21">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>127.09999999999997</v>
       </c>
+      <c r="AK9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AL9" s="19">
+        <f>AL4-AL6</f>
+        <v>4.6000000000000014</v>
+      </c>
+      <c r="AM9" s="20">
+        <f t="shared" ref="AM9:AQ9" si="18">AM4-AM6</f>
+        <v>8.3500000000000014</v>
+      </c>
+      <c r="AN9" s="20">
+        <f t="shared" si="18"/>
+        <v>14.599999999999994</v>
+      </c>
+      <c r="AO9" s="20">
+        <f t="shared" si="18"/>
+        <v>27.099999999999994</v>
+      </c>
+      <c r="AP9" s="20">
+        <f t="shared" si="18"/>
+        <v>64.599999999999966</v>
+      </c>
+      <c r="AQ9" s="21">
+        <f t="shared" si="18"/>
+        <v>127.10000000000002</v>
+      </c>
+      <c r="AT9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AU9" s="19">
+        <f>AU4-AU6</f>
+        <v>0</v>
+      </c>
+      <c r="AV9" s="20">
+        <f t="shared" ref="AV9:AZ9" si="19">AV4-AV6</f>
+        <v>0</v>
+      </c>
+      <c r="AW9" s="20">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AX9" s="20">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AY9" s="20">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AZ9" s="21">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>21</v>
       </c>
@@ -8999,23 +13099,23 @@
         <v>2.423</v>
       </c>
       <c r="C10" s="23">
-        <f t="shared" ref="C10:G10" si="16">C2-C7</f>
+        <f t="shared" ref="C10:G10" si="20">C2-C7</f>
         <v>3.6013999999999995</v>
       </c>
       <c r="D10" s="23">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>5.5654000000000003</v>
       </c>
       <c r="E10" s="23">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>9.4932000000000016</v>
       </c>
       <c r="F10" s="23">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>21.276899999999998</v>
       </c>
       <c r="G10" s="24">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>40.916499999999999</v>
       </c>
       <c r="J10" s="4" t="s">
@@ -9026,23 +13126,23 @@
         <v>2.4230999999999998</v>
       </c>
       <c r="L10" s="23">
-        <f t="shared" ref="L10:P10" si="17">L2-L7</f>
+        <f t="shared" ref="L10:P10" si="21">L2-L7</f>
         <v>3.6015000000000001</v>
       </c>
       <c r="M10" s="23">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>5.5653999999999995</v>
       </c>
       <c r="N10" s="23">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>9.4932999999999996</v>
       </c>
       <c r="O10" s="23">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>21.276999999999997</v>
       </c>
       <c r="P10" s="24">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>40.916399999999996</v>
       </c>
       <c r="S10" s="3" t="s">
@@ -9053,23 +13153,23 @@
         <v>3.8923000000000005</v>
       </c>
       <c r="U10" s="20">
-        <f t="shared" ref="U10:Y10" si="18">U2-U7</f>
+        <f t="shared" ref="U10:Y10" si="22">U2-U7</f>
         <v>6.9908999999999999</v>
       </c>
       <c r="V10" s="20">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>12.1555</v>
       </c>
       <c r="W10" s="20">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>22.484399999999997</v>
       </c>
       <c r="X10" s="20">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>53.471400000000003</v>
       </c>
       <c r="Y10" s="21">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>105.1164</v>
       </c>
       <c r="AB10" s="4" t="s">
@@ -9080,27 +13180,81 @@
         <v>3.8922999999999996</v>
       </c>
       <c r="AD10" s="23">
-        <f t="shared" ref="AD10:AH10" si="19">AD2-AD7</f>
+        <f t="shared" ref="AD10:AH10" si="23">AD2-AD7</f>
         <v>6.9909999999999997</v>
       </c>
       <c r="AE10" s="23">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>12.1554</v>
       </c>
       <c r="AF10" s="23">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>22.484500000000001</v>
       </c>
       <c r="AG10" s="23">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>53.471499999999992</v>
       </c>
       <c r="AH10" s="24">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>105.1164</v>
       </c>
+      <c r="AK10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="AL10" s="22">
+        <f>AL2-AL7</f>
+        <v>3.8923000000000005</v>
+      </c>
+      <c r="AM10" s="23">
+        <f t="shared" ref="AM10:AQ10" si="24">AM2-AM7</f>
+        <v>6.9908999999999999</v>
+      </c>
+      <c r="AN10" s="23">
+        <f t="shared" si="24"/>
+        <v>12.1555</v>
+      </c>
+      <c r="AO10" s="23">
+        <f t="shared" si="24"/>
+        <v>22.484400000000001</v>
+      </c>
+      <c r="AP10" s="23">
+        <f t="shared" si="24"/>
+        <v>53.471399999999996</v>
+      </c>
+      <c r="AQ10" s="24">
+        <f t="shared" si="24"/>
+        <v>105.1164</v>
+      </c>
+      <c r="AT10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="AU10" s="22">
+        <f>AU2-AU7</f>
+        <v>0</v>
+      </c>
+      <c r="AV10" s="23">
+        <f t="shared" ref="AV10:AZ10" si="25">AV2-AV7</f>
+        <v>0</v>
+      </c>
+      <c r="AW10" s="23">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="AX10" s="23">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="AY10" s="23">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="AZ10" s="24">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>9</v>
       </c>
@@ -9109,23 +13263,23 @@
         <v>3.0666666666666664</v>
       </c>
       <c r="C11" s="26">
-        <f t="shared" ref="C11:G11" si="20">2/3*2.3*C1</f>
+        <f t="shared" ref="C11:G11" si="26">2/3*2.3*C1</f>
         <v>7.6666666666666661</v>
       </c>
       <c r="D11" s="26">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>15.333333333333332</v>
       </c>
       <c r="E11" s="26">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>30.666666666666664</v>
       </c>
       <c r="F11" s="26">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>76.666666666666657</v>
       </c>
       <c r="G11" s="27">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>153.33333333333331</v>
       </c>
       <c r="J11" s="15" t="s">
@@ -9136,23 +13290,23 @@
         <v>6.1333333333333329</v>
       </c>
       <c r="L11" s="26">
-        <f t="shared" ref="L11:P11" si="21">2/3*2.3*L1*2</f>
+        <f t="shared" ref="L11:P11" si="27">2/3*2.3*L1*2</f>
         <v>15.333333333333332</v>
       </c>
       <c r="M11" s="26">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>30.666666666666664</v>
       </c>
       <c r="N11" s="26">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>61.333333333333329</v>
       </c>
       <c r="O11" s="26">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>153.33333333333331</v>
       </c>
       <c r="P11" s="27">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>306.66666666666663</v>
       </c>
       <c r="S11" s="14" t="s">
@@ -9163,23 +13317,23 @@
         <v>3.0666666666666664</v>
       </c>
       <c r="U11" s="26">
-        <f t="shared" ref="U11:Y11" si="22">2/3*2.3*U1*1</f>
+        <f t="shared" ref="U11:Y11" si="28">2/3*2.3*U1*1</f>
         <v>7.6666666666666661</v>
       </c>
       <c r="V11" s="26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>15.333333333333332</v>
       </c>
       <c r="W11" s="26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>30.666666666666664</v>
       </c>
       <c r="X11" s="26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>76.666666666666657</v>
       </c>
       <c r="Y11" s="27">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>153.33333333333331</v>
       </c>
       <c r="AB11" s="15" t="s">
@@ -9190,27 +13344,81 @@
         <v>6.1333333333333329</v>
       </c>
       <c r="AD11" s="26">
-        <f t="shared" ref="AD11:AH11" si="23">2/3*2.3*AD1*2</f>
+        <f t="shared" ref="AD11:AH11" si="29">2/3*2.3*AD1*2</f>
         <v>15.333333333333332</v>
       </c>
       <c r="AE11" s="26">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>30.666666666666664</v>
       </c>
       <c r="AF11" s="26">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>61.333333333333329</v>
       </c>
       <c r="AG11" s="26">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>153.33333333333331</v>
       </c>
       <c r="AH11" s="27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="29"/>
         <v>306.66666666666663</v>
       </c>
+      <c r="AK11" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="AL11" s="25">
+        <f>2/3*2.3*AL1*4</f>
+        <v>12.266666666666666</v>
+      </c>
+      <c r="AM11" s="25">
+        <f t="shared" ref="AM11:AQ11" si="30">2/3*2.3*AM1*4</f>
+        <v>30.666666666666664</v>
+      </c>
+      <c r="AN11" s="25">
+        <f t="shared" si="30"/>
+        <v>61.333333333333329</v>
+      </c>
+      <c r="AO11" s="25">
+        <f t="shared" si="30"/>
+        <v>122.66666666666666</v>
+      </c>
+      <c r="AP11" s="25">
+        <f t="shared" si="30"/>
+        <v>306.66666666666663</v>
+      </c>
+      <c r="AQ11" s="25">
+        <f t="shared" si="30"/>
+        <v>613.33333333333326</v>
+      </c>
+      <c r="AT11" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="AU11" s="25">
+        <f>2/3*2.3*AU1*4</f>
+        <v>12.266666666666666</v>
+      </c>
+      <c r="AV11" s="25">
+        <f t="shared" ref="AV11:AZ11" si="31">2/3*2.3*AV1*4</f>
+        <v>30.666666666666664</v>
+      </c>
+      <c r="AW11" s="25">
+        <f t="shared" si="31"/>
+        <v>61.333333333333329</v>
+      </c>
+      <c r="AX11" s="25">
+        <f t="shared" si="31"/>
+        <v>122.66666666666666</v>
+      </c>
+      <c r="AY11" s="25">
+        <f t="shared" si="31"/>
+        <v>306.66666666666663</v>
+      </c>
+      <c r="AZ11" s="25">
+        <f t="shared" si="31"/>
+        <v>613.33333333333326</v>
+      </c>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="B34" s="5" t="s">
         <v>10</v>
@@ -9239,8 +13447,22 @@
       <c r="AD34" s="7" t="s">
         <v>11</v>
       </c>
+      <c r="AK34" s="5"/>
+      <c r="AL34" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AM34" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="AT34" s="5"/>
+      <c r="AU34" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AV34" s="7" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>4</v>
       </c>
@@ -9277,8 +13499,22 @@
       <c r="AD35" s="9">
         <v>0</v>
       </c>
+      <c r="AK35" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AL35" s="8">
+        <v>6.633</v>
+      </c>
+      <c r="AM35" s="9">
+        <v>0</v>
+      </c>
+      <c r="AT35" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AU35" s="8"/>
+      <c r="AV35" s="9"/>
     </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>5</v>
       </c>
@@ -9315,8 +13551,22 @@
       <c r="AD36" s="11">
         <v>0</v>
       </c>
+      <c r="AK36" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AL36" s="10">
+        <v>0.50600000000000001</v>
+      </c>
+      <c r="AM36" s="11">
+        <v>0</v>
+      </c>
+      <c r="AT36" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AU36" s="10"/>
+      <c r="AV36" s="11"/>
     </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>6</v>
       </c>
@@ -9353,8 +13603,22 @@
       <c r="AD37" s="11">
         <v>0</v>
       </c>
+      <c r="AK37" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AL37" s="10">
+        <v>0.11</v>
+      </c>
+      <c r="AM37" s="11">
+        <v>0</v>
+      </c>
+      <c r="AT37" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AU37" s="10"/>
+      <c r="AV37" s="11"/>
     </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>7</v>
       </c>
@@ -9391,8 +13655,22 @@
       <c r="AD38" s="11">
         <v>2.1</v>
       </c>
+      <c r="AK38" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AL38" s="10">
+        <v>1.25</v>
+      </c>
+      <c r="AM38" s="11">
+        <v>2.1</v>
+      </c>
+      <c r="AT38" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AU38" s="10"/>
+      <c r="AV38" s="11"/>
     </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>8</v>
       </c>
@@ -9429,6 +13707,20 @@
       <c r="AD39" s="13">
         <v>1.8260000000000001</v>
       </c>
+      <c r="AK39" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AL39" s="12">
+        <v>1.0329999999999999</v>
+      </c>
+      <c r="AM39" s="13">
+        <v>1.8260000000000001</v>
+      </c>
+      <c r="AT39" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU39" s="12"/>
+      <c r="AV39" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>